<commit_message>
Add short title to simple route mapping test file
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application.IntegrationTests/QualificationRoutePathMapping/RoutePathMapping-Simple.xlsx
+++ b/src/Sfa.Tl.Matching.Application.IntegrationTests/QualificationRoutePathMapping/RoutePathMapping-Simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike\Downloads\TL_TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esfa\tl-matching\src\Sfa.Tl.Matching.Application.IntegrationTests\QualificationRoutePathMapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B43D1A-0CBF-4292-8B9B-3E3BFCBE162C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE018FA9-4D77-41F2-860C-614AE4496E59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4943" yWindow="907" windowWidth="18224" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Quals" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Science</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Short Title</t>
+  </si>
+  <si>
+    <t>L3 AGCE Art and Design</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L24" sqref="L24"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
@@ -924,6 +927,9 @@
       <c r="B4" t="s">
         <v>36</v>
       </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>

</xml_diff>

<commit_message>
Add validation of path id columns of Source column.
Changed column names in QualificationRoutePathMappingFileImportDto to match database.
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application.IntegrationTests/QualificationRoutePathMapping/RoutePathMapping-Simple.xlsx
+++ b/src/Sfa.Tl.Matching.Application.IntegrationTests/QualificationRoutePathMapping/RoutePathMapping-Simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esfa\tl-matching\src\Sfa.Tl.Matching.Application.IntegrationTests\QualificationRoutePathMapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE018FA9-4D77-41F2-860C-614AE4496E59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7A329-BF37-4537-AAD9-24C4EE7B11E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2543" yWindow="2543" windowWidth="19125" windowHeight="12494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Quals" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Science</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>L3 AGCE Art and Design</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Gatsby</t>
   </si>
 </sst>
 </file>
@@ -619,12 +625,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L24" sqref="L24"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
@@ -658,7 +664,7 @@
     <col min="37" max="38" width="4.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.4">
+    <row r="1" spans="1:39" ht="15.4">
       <c r="D1" s="14" t="s">
         <v>38</v>
       </c>
@@ -697,7 +703,7 @@
       <c r="AK1" s="15"/>
       <c r="AL1" s="15"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:39">
       <c r="D2" s="6">
         <v>2</v>
       </c>
@@ -804,7 +810,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="1" customFormat="1" ht="222" customHeight="1">
+    <row r="3" spans="1:39" s="1" customFormat="1" ht="222" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -919,8 +925,11 @@
       <c r="AL3" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="AM3" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4">
         <v>60144567</v>
       </c>
@@ -949,6 +958,9 @@
       <c r="AB4"/>
       <c r="AH4" s="4">
         <v>31</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>